<commit_message>
Finalize BOM, add all footprints
</commit_message>
<xml_diff>
--- a/pcb/7001-mainboard/7001-ventilator_mainboard.xlsx
+++ b/pcb/7001-mainboard/7001-ventilator_mainboard.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="203">
   <si>
     <t xml:space="preserve">Sync</t>
   </si>
@@ -100,6 +100,21 @@
     <t xml:space="preserve">4.7k</t>
   </si>
   <si>
+    <t xml:space="preserve">RV1,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Varistor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jitter_Footprints:WE_VS_Varistor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">82551250</t>
+  </si>
+  <si>
     <t xml:space="preserve">R10, R12, R6, R32, R39,</t>
   </si>
   <si>
@@ -247,12 +262,12 @@
     <t xml:space="preserve">D3,</t>
   </si>
   <si>
-    <t xml:space="preserve">1</t>
-  </si>
-  <si>
     <t xml:space="preserve">S5MB R5G 100V</t>
   </si>
   <si>
+    <t xml:space="preserve">Diode_SMD:D_SMB</t>
+  </si>
+  <si>
     <t xml:space="preserve">S5MB R5G</t>
   </si>
   <si>
@@ -262,16 +277,13 @@
     <t xml:space="preserve">D_TVS</t>
   </si>
   <si>
+    <t xml:space="preserve">Jitter_Footprints:WE-TVSP_TVS_DIODE</t>
+  </si>
+  <si>
     <t xml:space="preserve">824501301</t>
   </si>
   <si>
-    <t xml:space="preserve">RV1,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Varistor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">82551250</t>
+    <t xml:space="preserve">2536572</t>
   </si>
   <si>
     <t xml:space="preserve">D9, D8, D7, D6,</t>
@@ -307,6 +319,9 @@
     <t xml:space="preserve">744282010</t>
   </si>
   <si>
+    <t xml:space="preserve">Jitter_Footprints:L_CommonMode_Wuerth_WE-SCC</t>
+  </si>
+  <si>
     <t xml:space="preserve">J1,</t>
   </si>
   <si>
@@ -361,7 +376,10 @@
     <t xml:space="preserve">Raspberry_Pi_2_3</t>
   </si>
   <si>
-    <t xml:space="preserve">610020243021</t>
+    <t xml:space="preserve">Jitter_Footprints:PinSocket_2x20_P2.54mm_Vertical_holes_SMD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REF-182665-01</t>
   </si>
   <si>
     <t xml:space="preserve">2827937</t>
@@ -601,13 +619,16 @@
     <t xml:space="preserve">732-2753-ND </t>
   </si>
   <si>
-    <t xml:space="preserve">TODO</t>
+    <t xml:space="preserve">K9</t>
   </si>
   <si>
     <t xml:space="preserve">20-pin tussenheader RPI</t>
   </si>
   <si>
-    <t xml:space="preserve">Standaard 20-pin 2-row 2.54mm pitch through hole header?</t>
+    <t xml:space="preserve">wordt tijdens assemblage tussen pcb en RPI geplaatst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REF-182683-02</t>
   </si>
 </sst>
 </file>
@@ -657,7 +678,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -674,12 +695,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF00F200"/>
         <bgColor rgb="FF33CCCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF20000"/>
-        <bgColor rgb="FF800000"/>
       </patternFill>
     </fill>
   </fills>
@@ -717,7 +732,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -754,15 +769,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -783,7 +790,7 @@
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFF20000"/>
+      <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00F200"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFF200"/>
@@ -849,8 +856,8 @@
   </sheetPr>
   <dimension ref="A1:J1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F26" activeCellId="0" sqref="F26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D56" activeCellId="0" sqref="D56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1048,24 +1055,24 @@
       <c r="A8" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="7" t="s">
         <v>27</v>
       </c>
       <c r="D8" s="1" t="n">
         <f aca="false">C8*5</f>
-        <v>25</v>
-      </c>
-      <c r="E8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H8" s="2" t="n">
-        <v>2447553</v>
+      <c r="F8" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1073,47 +1080,47 @@
         <v>1</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D9" s="1" t="n">
         <f aca="false">C9*5</f>
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H9" s="2" t="n">
-        <v>2447706</v>
+        <v>2447553</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" s="2" t="n">
-        <v>2</v>
+      <c r="B10" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>35</v>
       </c>
       <c r="D10" s="1" t="n">
         <f aca="false">C10*5</f>
         <v>10</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H10" s="2" t="n">
-        <v>2447551</v>
+        <v>2447706</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1121,7 +1128,7 @@
         <v>1</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C11" s="2" t="n">
         <v>2</v>
@@ -1131,13 +1138,13 @@
         <v>10</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>37</v>
+        <v>13</v>
+      </c>
+      <c r="H11" s="2" t="n">
+        <v>2447551</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1145,7 +1152,7 @@
         <v>1</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C12" s="2" t="n">
         <v>2</v>
@@ -1155,13 +1162,13 @@
         <v>10</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H12" s="2" t="n">
-        <v>2409053</v>
+        <v>41</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1169,23 +1176,23 @@
         <v>1</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C13" s="2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D13" s="1" t="n">
         <f aca="false">C13*5</f>
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E13" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F13" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="H13" s="2" t="n">
-        <v>1414681</v>
+        <v>2409053</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1193,23 +1200,23 @@
         <v>1</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C14" s="2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D14" s="1" t="n">
         <f aca="false">C14*5</f>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="H14" s="2" t="n">
-        <v>3013468</v>
+        <v>1414681</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1217,7 +1224,7 @@
         <v>1</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C15" s="2" t="n">
         <v>2</v>
@@ -1227,61 +1234,61 @@
         <v>10</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="H15" s="2" t="n">
-        <v>1414681</v>
+        <v>3013468</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B16" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>30</v>
+      <c r="B16" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" s="2" t="n">
+        <v>2</v>
       </c>
       <c r="D16" s="1" t="n">
         <f aca="false">C16*5</f>
         <v>10</v>
       </c>
-      <c r="E16" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="G16" s="8" t="s">
-        <v>49</v>
+      <c r="E16" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H16" s="2" t="n">
+        <v>1414681</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B17" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>20</v>
+      <c r="B17" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>35</v>
       </c>
       <c r="D17" s="1" t="n">
         <f aca="false">C17*5</f>
-        <v>15</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H17" s="2" t="n">
-        <v>1650861</v>
+        <v>10</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1289,44 +1296,44 @@
         <v>1</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>53</v>
+        <v>20</v>
       </c>
       <c r="D18" s="1" t="n">
         <f aca="false">C18*5</f>
-        <v>75</v>
+        <v>15</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="H18" s="2" t="n">
-        <v>1650866</v>
+        <v>1650861</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C19" s="2" t="n">
-        <v>5</v>
+      <c r="B19" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>58</v>
       </c>
       <c r="D19" s="1" t="n">
         <f aca="false">C19*5</f>
-        <v>25</v>
+        <v>75</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="H19" s="2" t="n">
         <v>1650866</v>
@@ -1337,23 +1344,23 @@
         <v>1</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C20" s="2" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D20" s="1" t="n">
         <f aca="false">C20*5</f>
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="H20" s="2" t="n">
-        <v>2688485</v>
+        <v>1650866</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1361,23 +1368,23 @@
         <v>1</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="C21" s="2" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D21" s="1" t="n">
         <f aca="false">C21*5</f>
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="H21" s="2" t="n">
-        <v>2346968</v>
+        <v>2688485</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1385,23 +1392,23 @@
         <v>1</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="C22" s="2" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D22" s="1" t="n">
         <f aca="false">C22*5</f>
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="H22" s="2" t="n">
-        <v>3013485</v>
+        <v>2346968</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1409,23 +1416,23 @@
         <v>1</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C23" s="2" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D23" s="1" t="n">
         <f aca="false">C23*5</f>
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="H23" s="2" t="n">
-        <v>2834943</v>
+        <v>3013485</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1433,26 +1440,23 @@
         <v>1</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C24" s="2" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D24" s="1" t="n">
         <f aca="false">C24*5</f>
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H24" s="2" t="n">
-        <v>2859824</v>
+        <v>2834943</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1460,89 +1464,104 @@
         <v>1</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C25" s="2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D25" s="1" t="n">
         <f aca="false">C25*5</f>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H25" s="2" t="n">
-        <v>3003750</v>
+        <v>2859824</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="B26" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="C26" s="9" t="s">
+      <c r="A26" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>75</v>
+      </c>
+      <c r="C26" s="2" t="n">
+        <v>2</v>
       </c>
       <c r="D26" s="1" t="n">
         <f aca="false">C26*5</f>
-        <v>5</v>
-      </c>
-      <c r="E26" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E26" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="G26" s="9" t="s">
+      <c r="F26" s="1" t="s">
         <v>77</v>
       </c>
+      <c r="G26" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="H26" s="2" t="n">
+        <v>3003750</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="B27" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>20</v>
+      <c r="A27" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>27</v>
       </c>
       <c r="D27" s="1" t="n">
         <f aca="false">C27*5</f>
-        <v>15</v>
-      </c>
-      <c r="E27" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="G27" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E27" s="7" t="s">
         <v>80</v>
       </c>
+      <c r="F27" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="G27" s="7" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="9" t="n">
+      <c r="A28" s="1" t="n">
         <v>1</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>75</v>
+        <v>20</v>
       </c>
       <c r="D28" s="1" t="n">
         <f aca="false">C28*5</f>
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="G28" s="8" t="s">
-        <v>83</v>
+        <v>84</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="G28" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="H28" s="7" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1550,7 +1569,7 @@
         <v>1</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="C29" s="7" t="s">
         <v>17</v>
@@ -1560,16 +1579,16 @@
         <v>20</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="G29" s="8" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="H29" s="7" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1577,47 +1596,50 @@
         <v>1</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>75</v>
+        <v>27</v>
       </c>
       <c r="D30" s="1" t="n">
         <f aca="false">C30*5</f>
         <v>5</v>
       </c>
       <c r="E30" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F30" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="F30" s="7" t="s">
-        <v>86</v>
-      </c>
       <c r="G30" s="8" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="H30" s="7" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="B31" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="C31" s="9" t="s">
-        <v>75</v>
+      <c r="A31" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>27</v>
       </c>
       <c r="D31" s="1" t="n">
         <f aca="false">C31*5</f>
         <v>5</v>
       </c>
-      <c r="E31" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="G31" s="9" t="s">
-        <v>94</v>
+      <c r="E31" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="F31" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="G31" s="7" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1625,7 +1647,7 @@
         <v>1</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="C32" s="2" t="n">
         <v>1</v>
@@ -1635,45 +1657,45 @@
         <v>5</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="H32" s="2" t="n">
         <v>1568026</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="n">
         <v>1</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>75</v>
+        <v>27</v>
       </c>
       <c r="D33" s="1" t="n">
         <f aca="false">C33*5</f>
         <v>5</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="n">
         <v>1</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="C34" s="2" t="n">
         <v>1</v>
@@ -1683,18 +1705,18 @@
         <v>5</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="n">
         <v>1</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="C35" s="2" t="n">
         <v>1</v>
@@ -1704,31 +1726,31 @@
         <v>5</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="n">
         <v>1</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D36" s="1" t="n">
         <f aca="false">C36*5</f>
         <v>25</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="G36" s="2" t="n">
         <v>691322110002</v>
@@ -1738,123 +1760,126 @@
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="B37" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="C37" s="9" t="s">
-        <v>75</v>
+      <c r="A37" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>27</v>
       </c>
       <c r="D37" s="1" t="n">
         <f aca="false">C37*5</f>
         <v>5</v>
       </c>
-      <c r="E37" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="G37" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="H37" s="9" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E37" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="F37" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="G37" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="H37" s="7" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="n">
         <v>1</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>75</v>
+        <v>27</v>
       </c>
       <c r="D38" s="1" t="n">
         <f aca="false">C38*5</f>
         <v>5</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="n">
         <v>1</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D39" s="1" t="n">
         <f aca="false">C39*5</f>
         <v>10</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="16.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="n">
         <v>1</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>75</v>
+        <v>27</v>
       </c>
       <c r="D40" s="1" t="n">
         <f aca="false">C40*5</f>
         <v>5</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="G40" s="8" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="16.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="n">
         <v>1</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>75</v>
+        <v>27</v>
       </c>
       <c r="D41" s="1" t="n">
         <f aca="false">C41*5</f>
         <v>5</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="G41" s="8" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1862,26 +1887,26 @@
         <v>1</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>75</v>
+        <v>27</v>
       </c>
       <c r="D42" s="1" t="n">
         <f aca="false">C42*5</f>
         <v>5</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1889,7 +1914,7 @@
         <v>1</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="C43" s="2" t="n">
         <v>2</v>
@@ -1899,16 +1924,16 @@
         <v>10</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="J43" s="1" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1916,7 +1941,7 @@
         <v>1</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="C44" s="2" t="n">
         <v>1</v>
@@ -1926,13 +1951,13 @@
         <v>5</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="H44" s="2" t="n">
         <v>3116500</v>
@@ -1943,7 +1968,7 @@
         <v>1</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="C45" s="2" t="n">
         <v>1</v>
@@ -1953,13 +1978,13 @@
         <v>5</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="H45" s="2" t="n">
         <v>2115662</v>
@@ -1970,7 +1995,7 @@
         <v>1</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="C46" s="2" t="n">
         <v>1</v>
@@ -1980,13 +2005,13 @@
         <v>5</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="H46" s="2" t="n">
         <v>1578404</v>
@@ -1997,26 +2022,26 @@
         <v>1</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>75</v>
+        <v>27</v>
       </c>
       <c r="D47" s="1" t="n">
         <f aca="false">C47*5</f>
         <v>5</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2024,7 +2049,7 @@
         <v>1</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="C48" s="2" t="n">
         <v>1</v>
@@ -2034,24 +2059,24 @@
         <v>5</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="H48" s="2" t="n">
         <v>3007529</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="n">
         <v>1</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="C49" s="2" t="n">
         <v>1</v>
@@ -2061,24 +2086,24 @@
         <v>5</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="H49" s="2" t="n">
         <v>1827275</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="n">
         <v>1</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="C50" s="2" t="n">
         <v>2</v>
@@ -2088,24 +2113,24 @@
         <v>10</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="I50" s="10" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>168</v>
+      </c>
+      <c r="I50" s="9" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="n">
         <v>1</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="C51" s="2" t="n">
         <v>2</v>
@@ -2115,27 +2140,27 @@
         <v>10</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="I51" s="10" t="s">
-        <v>168</v>
+        <v>172</v>
+      </c>
+      <c r="I51" s="9" t="s">
+        <v>174</v>
       </c>
       <c r="J51" s="1" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="n">
         <v>1</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="C52" s="2" t="n">
         <v>2</v>
@@ -2145,13 +2170,13 @@
         <v>10</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="H52" s="2" t="n">
         <v>1440816</v>
@@ -2162,7 +2187,7 @@
         <v>1</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="C53" s="2" t="n">
         <v>1</v>
@@ -2172,13 +2197,13 @@
         <v>5</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
       <c r="H53" s="2" t="n">
         <v>2308719</v>
@@ -2188,16 +2213,15 @@
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="3"/>
       <c r="B58" s="3" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="11"/>
+        <v>183</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B59" s="1" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="C59" s="2" t="n">
         <v>5</v>
@@ -2207,22 +2231,21 @@
         <v>25</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="G59" s="12" t="s">
-        <v>181</v>
+        <v>186</v>
+      </c>
+      <c r="G59" s="10" t="s">
+        <v>187</v>
       </c>
       <c r="J59" s="1" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="11"/>
+        <v>188</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B60" s="1" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="C60" s="2" t="n">
         <v>2</v>
@@ -2232,22 +2255,21 @@
         <v>10</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="G60" s="12" t="s">
-        <v>186</v>
+        <v>191</v>
+      </c>
+      <c r="G60" s="10" t="s">
+        <v>192</v>
       </c>
       <c r="J60" s="1" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="11"/>
+        <v>193</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B61" s="1" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="C61" s="2" t="n">
         <v>1</v>
@@ -2257,22 +2279,21 @@
         <v>5</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="G61" s="12" t="s">
-        <v>191</v>
+        <v>196</v>
+      </c>
+      <c r="G61" s="10" t="s">
+        <v>197</v>
       </c>
       <c r="J61" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="11"/>
+        <v>198</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B62" s="1" t="s">
-        <v>193</v>
+        <v>199</v>
       </c>
       <c r="C62" s="2" t="n">
         <v>1</v>
@@ -2282,12 +2303,20 @@
         <v>5</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>195</v>
-      </c>
-    </row>
+        <v>201</v>
+      </c>
+      <c r="G62" s="2" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="1048544" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048545" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048546" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048547" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048548" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048549" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048550" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048551" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2300,11 +2329,11 @@
     <row r="1048558" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048559" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048560" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048561" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048562" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048563" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048564" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048565" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048561" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048562" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
PCB: final BOM (1x 100nf removed)
</commit_message>
<xml_diff>
--- a/pcb/7001-mainboard/7001-ventilator_mainboard.xlsx
+++ b/pcb/7001-mainboard/7001-ventilator_mainboard.xlsx
@@ -193,10 +193,10 @@
     <t xml:space="preserve">10nF</t>
   </si>
   <si>
-    <t xml:space="preserve">C1, C3, C2, C15, C26, C28, C29, C40, C43, C49, C50, C8, C31, C9, C33,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15</t>
+    <t xml:space="preserve">C1, C3, C2, C15, C26, C28, C29, C40, C43, C49, C8, C31, C9, C33,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14</t>
   </si>
   <si>
     <t xml:space="preserve">100nF</t>
@@ -241,7 +241,7 @@
     <t xml:space="preserve">330uF</t>
   </si>
   <si>
-    <t xml:space="preserve">Jitter_Footprints:CP_Elec_12.5x13.5</t>
+    <t xml:space="preserve">Jitter_Footprints:CP_Elec_12.5_MAL214699107E3</t>
   </si>
   <si>
     <t xml:space="preserve">MAL214699107E3</t>
@@ -328,7 +328,7 @@
     <t xml:space="preserve">USB_B_Micro</t>
   </si>
   <si>
-    <t xml:space="preserve">Connector_USB:USB_Micro-B_Molex_47346-0001</t>
+    <t xml:space="preserve">Jitter_Footprints:USB_Micro-B_Molex_47346-0001</t>
   </si>
   <si>
     <t xml:space="preserve">47346-0001</t>
@@ -678,7 +678,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -695,6 +695,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF00F200"/>
         <bgColor rgb="FF33CCCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF20000"/>
+        <bgColor rgb="FF800000"/>
       </patternFill>
     </fill>
   </fills>
@@ -732,7 +738,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -769,7 +775,15 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -790,7 +804,7 @@
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FFF20000"/>
       <rgbColor rgb="FF00F200"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFF200"/>
@@ -856,8 +870,8 @@
   </sheetPr>
   <dimension ref="A1:J1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D56" activeCellId="0" sqref="D56"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2:D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1327,7 +1341,7 @@
       </c>
       <c r="D19" s="1" t="n">
         <f aca="false">C19*5</f>
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>59</v>
@@ -1476,7 +1490,7 @@
       <c r="E25" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="F25" s="1" t="s">
+      <c r="F25" s="9" t="s">
         <v>73</v>
       </c>
       <c r="G25" s="2" t="s">
@@ -1642,7 +1656,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="n">
         <v>1</v>
       </c>
@@ -1659,7 +1673,7 @@
       <c r="E32" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="F32" s="1" t="s">
+      <c r="F32" s="5" t="s">
         <v>102</v>
       </c>
       <c r="G32" s="2" t="s">
@@ -1669,7 +1683,7 @@
         <v>1568026</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="n">
         <v>1</v>
       </c>
@@ -1711,7 +1725,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="n">
         <v>1</v>
       </c>
@@ -1807,7 +1821,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="16.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="n">
         <v>1</v>
       </c>
@@ -1858,7 +1872,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="16.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="n">
         <v>1</v>
       </c>
@@ -1936,7 +1950,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="16.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="n">
         <v>1</v>
       </c>
@@ -1990,7 +2004,7 @@
         <v>2115662</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="16.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="n">
         <v>1</v>
       </c>
@@ -2121,7 +2135,7 @@
       <c r="G50" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="I50" s="9" t="s">
+      <c r="I50" s="10" t="s">
         <v>170</v>
       </c>
     </row>
@@ -2148,7 +2162,7 @@
       <c r="G51" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="I51" s="9" t="s">
+      <c r="I51" s="10" t="s">
         <v>174</v>
       </c>
       <c r="J51" s="1" t="s">
@@ -2220,6 +2234,7 @@
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A59" s="11"/>
       <c r="B59" s="1" t="s">
         <v>184</v>
       </c>
@@ -2227,64 +2242,66 @@
         <v>5</v>
       </c>
       <c r="D59" s="1" t="n">
+        <f aca="false">C58*5</f>
+        <v>0</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="G59" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="J59" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A60" s="11"/>
+      <c r="B60" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="C60" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D60" s="1" t="n">
         <f aca="false">C59*5</f>
         <v>25</v>
       </c>
-      <c r="E59" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="F59" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="G59" s="10" t="s">
-        <v>187</v>
-      </c>
-      <c r="J59" s="1" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B60" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="C60" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="D60" s="1" t="n">
+      <c r="E60" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="G60" s="12" t="s">
+        <v>192</v>
+      </c>
+      <c r="J60" s="1" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A61" s="11"/>
+      <c r="B61" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C61" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D61" s="1" t="n">
         <f aca="false">C60*5</f>
         <v>10</v>
       </c>
-      <c r="E60" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="F60" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="G60" s="10" t="s">
-        <v>192</v>
-      </c>
-      <c r="J60" s="1" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B61" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="C61" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D61" s="1" t="n">
-        <f aca="false">C61*5</f>
-        <v>5</v>
-      </c>
       <c r="E61" s="1" t="s">
         <v>195</v>
       </c>
       <c r="F61" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="G61" s="10" t="s">
+      <c r="G61" s="12" t="s">
         <v>197</v>
       </c>
       <c r="J61" s="1" t="s">
@@ -2292,6 +2309,7 @@
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A62" s="11"/>
       <c r="B62" s="1" t="s">
         <v>199</v>
       </c>
@@ -2299,7 +2317,7 @@
         <v>1</v>
       </c>
       <c r="D62" s="1" t="n">
-        <f aca="false">C62*5</f>
+        <f aca="false">C61*5</f>
         <v>5</v>
       </c>
       <c r="E62" s="1" t="s">
@@ -2312,6 +2330,7 @@
         <v>202</v>
       </c>
     </row>
+    <row r="1048543" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048544" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048545" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048546" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2328,7 +2347,7 @@
     <row r="1048557" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048558" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048559" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048560" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048560" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048561" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048562" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
PCB layout: final locations and BOM (?)
</commit_message>
<xml_diff>
--- a/pcb/7001-mainboard/7001-ventilator_mainboard.xlsx
+++ b/pcb/7001-mainboard/7001-ventilator_mainboard.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="212">
   <si>
     <t xml:space="preserve">Sync</t>
   </si>
@@ -67,63 +67,72 @@
     <t xml:space="preserve">33R</t>
   </si>
   <si>
-    <t xml:space="preserve">R49, R50, R41, R42, R43, R47,</t>
+    <t xml:space="preserve">R49, R50, R41, R42, R43,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">150</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R3, R12, R22, R24, R23,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1k5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R29, R40, R38, R19, R44, R37, R46, R45,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.3k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R34, R36, R32, R21,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.7k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R47,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">150 1%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R48,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.32k 1%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.2k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RV1,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Varistor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jitter_Footprints:WE_VS_Varistor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">82551250</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R6, R35, R39, R15, R18, R11,</t>
   </si>
   <si>
     <t xml:space="preserve">6</t>
   </si>
   <si>
-    <t xml:space="preserve">150</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R11, R3, R12, R23, R22,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1k5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R29, R40, R38, R19, R44, R37, R46, R45,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.3k</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R34, R36, R32, R21,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4.7k</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R48,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.2k</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RV1,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Varistor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jitter_Footprints:WE_VS_Varistor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">82551250</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R6, R35, R39, R15, R18,</t>
-  </si>
-  <si>
     <t xml:space="preserve">10k</t>
   </si>
   <si>
@@ -193,22 +202,22 @@
     <t xml:space="preserve">885012208112</t>
   </si>
   <si>
-    <t xml:space="preserve">C28, C29, C1, C23, C49, C2, C3, C21, C15, C50, C8, C9, C31, C33,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14</t>
+    <t xml:space="preserve">C28, C29, C1, C23, C49, C2, C3, C21, C15, C50, C43, C8, C9, C31, C33,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15</t>
   </si>
   <si>
     <t xml:space="preserve">100nF</t>
   </si>
   <si>
-    <t xml:space="preserve">C19, C39, C48,</t>
+    <t xml:space="preserve">C19, C39, C48, C51, C54,</t>
   </si>
   <si>
     <t xml:space="preserve">100nF 50V</t>
   </si>
   <si>
-    <t xml:space="preserve">C11, C4, C30, C32,</t>
+    <t xml:space="preserve">C11, C4, C52, C30, C32,</t>
   </si>
   <si>
     <t xml:space="preserve">1uF</t>
@@ -220,7 +229,7 @@
     <t xml:space="preserve">4.7uF</t>
   </si>
   <si>
-    <t xml:space="preserve">C25, C16, C43,</t>
+    <t xml:space="preserve">C25, C16, C53,</t>
   </si>
   <si>
     <t xml:space="preserve">10uF</t>
@@ -349,6 +358,15 @@
     <t xml:space="preserve">J5,</t>
   </si>
   <si>
+    <t xml:space="preserve">5-pin screw terminal vertical</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jitter_Footprints:TerminalBlock_Wurth_WR-TBL_691321100005_1x05_P3.50mm_Vertical</t>
+  </si>
+  <si>
+    <t xml:space="preserve">691321100005</t>
+  </si>
+  <si>
     <t xml:space="preserve">2-pin screw terminal</t>
   </si>
   <si>
@@ -373,7 +391,7 @@
     <t xml:space="preserve">Connector_PinHeader_2.54mm:PinHeader_1x05_P2.54mm_Vertical</t>
   </si>
   <si>
-    <t xml:space="preserve">J7,</t>
+    <t xml:space="preserve">J7, J2,</t>
   </si>
   <si>
     <t xml:space="preserve">6-pin FFC connector</t>
@@ -415,6 +433,9 @@
     <t xml:space="preserve">J11, J8,</t>
   </si>
   <si>
+    <t xml:space="preserve">5-pin screw terminal</t>
+  </si>
+  <si>
     <t xml:space="preserve">Jitter_Footprints:TerminalBlock_Wurth_WR-TBL_691322110005_1x05_P3.50mm_Horizontal</t>
   </si>
   <si>
@@ -574,13 +595,13 @@
     <t xml:space="preserve">U16,</t>
   </si>
   <si>
-    <t xml:space="preserve">LD1086DT33TR</t>
+    <t xml:space="preserve">LD1086DTTR</t>
   </si>
   <si>
     <t xml:space="preserve">Package_TO_SOT_SMD:TO-252-2</t>
   </si>
   <si>
-    <t xml:space="preserve">1467774</t>
+    <t xml:space="preserve">LD1086DTTR (adjustable)</t>
   </si>
   <si>
     <t xml:space="preserve">Y1,</t>
@@ -598,10 +619,7 @@
     <t xml:space="preserve">Non-pcb parts</t>
   </si>
   <si>
-    <t xml:space="preserve">TODO: dit is niet up to date!</t>
-  </si>
-  <si>
-    <t xml:space="preserve">K7, K5, K3, K13, K14</t>
+    <t xml:space="preserve">K3, K4, K13, K14</t>
   </si>
   <si>
     <t xml:space="preserve">2 way straight</t>
@@ -616,34 +634,16 @@
     <t xml:space="preserve">732-2751-ND </t>
   </si>
   <si>
-    <t xml:space="preserve">K12, K8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3 way straight</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mates with 691322110003</t>
-  </si>
-  <si>
-    <t xml:space="preserve">691361100003</t>
-  </si>
-  <si>
-    <t xml:space="preserve">732-2752-ND </t>
-  </si>
-  <si>
-    <t xml:space="preserve">K11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4 way straight</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mates with 691322110004</t>
-  </si>
-  <si>
-    <t xml:space="preserve">691361100004</t>
-  </si>
-  <si>
-    <t xml:space="preserve">732-2753-ND </t>
+    <t xml:space="preserve">K5, K11, K8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 way straight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">691361100005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">732-2754-ND </t>
   </si>
   <si>
     <t xml:space="preserve">K9</t>
@@ -666,7 +666,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -698,6 +698,14 @@
       <charset val="1"/>
     </font>
     <font>
+      <strike val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="13"/>
       <color rgb="FF333333"/>
       <name val="Arial"/>
@@ -714,12 +722,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFF200"/>
-        <bgColor rgb="FFFFFF00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF00F200"/>
         <bgColor rgb="FF33CCCC"/>
       </patternFill>
@@ -728,6 +730,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFF20000"/>
         <bgColor rgb="FF800000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFF200"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -765,7 +773,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -790,19 +798,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -810,11 +814,27 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -895,10 +915,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I1048576"/>
+  <dimension ref="A1:J1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D68" activeCellId="0" sqref="D68"/>
+      <selection pane="topLeft" activeCell="B67" activeCellId="0" sqref="B67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -906,14 +926,14 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="5.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="49.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="4.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="21.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="25.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="74.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="18.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="21.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="8.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="27.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="13.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="10" style="1" width="8.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="1" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -949,10 +969,10 @@
       <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -969,7 +989,7 @@
       <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C3" s="2" t="n">
@@ -989,10 +1009,10 @@
       <c r="A4" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="2" t="s">
         <v>16</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -1009,14 +1029,14 @@
       <c r="A5" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>12</v>
@@ -1029,14 +1049,14 @@
       <c r="A6" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="D6" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>23</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>12</v>
@@ -1049,14 +1069,14 @@
       <c r="A7" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>25</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>12</v>
@@ -1069,16 +1089,16 @@
       <c r="A8" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="D8" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="5" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1086,177 +1106,170 @@
       <c r="A9" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" s="8" t="s">
+      <c r="E9" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="6"/>
+      <c r="B10" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="E9" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G10" s="2" t="n">
-        <v>2447553</v>
-      </c>
+      <c r="F10" s="7"/>
     </row>
     <row r="11" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>10</v>
+      <c r="B11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G11" s="2" t="n">
-        <v>2447706</v>
+        <v>33</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>38</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>12</v>
       </c>
       <c r="G12" s="2" t="n">
-        <v>2447551</v>
+        <v>2447553</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C13" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="E13" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>42</v>
+        <v>12</v>
+      </c>
+      <c r="G13" s="2" t="n">
+        <v>2447706</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B14" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>27</v>
+      <c r="B14" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>41</v>
+        <v>12</v>
       </c>
       <c r="G14" s="2" t="n">
-        <v>2409053</v>
+        <v>2447551</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G15" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G15" s="2" t="n">
-        <v>1414681</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C16" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="E16" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G16" s="2" t="n">
-        <v>3013468</v>
+        <v>2409053</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B17" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C17" s="6" t="s">
+      <c r="B17" s="1" t="s">
         <v>48</v>
       </c>
+      <c r="C17" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="D17" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G17" s="2" t="n">
         <v>1414681</v>
@@ -1266,80 +1279,80 @@
       <c r="A18" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C18" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="E18" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="F18" s="9" t="s">
-        <v>56</v>
+      <c r="E18" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G18" s="2" t="n">
+        <v>3013468</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B19" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>58</v>
+      <c r="B19" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>51</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G19" s="2" t="n">
-        <v>1650866</v>
+        <v>1414681</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B20" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>48</v>
+      <c r="B20" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>56</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G20" s="2" t="n">
-        <v>1650866</v>
+        <v>58</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C21" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>63</v>
-      </c>
       <c r="E21" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G21" s="2" t="n">
-        <v>2688485</v>
+        <v>1650866</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1347,59 +1360,59 @@
         <v>1</v>
       </c>
       <c r="B22" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C22" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>65</v>
-      </c>
       <c r="E22" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G22" s="2" t="n">
-        <v>2346968</v>
+        <v>1650866</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B23" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C23" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>67</v>
-      </c>
       <c r="E23" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G23" s="2" t="n">
-        <v>3013485</v>
+        <v>2688485</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C24" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C24" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>69</v>
-      </c>
       <c r="E24" s="1" t="s">
-        <v>70</v>
+        <v>44</v>
       </c>
       <c r="G24" s="2" t="n">
-        <v>2834943</v>
+        <v>2346968</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1407,177 +1420,174 @@
         <v>1</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C25" s="2" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>74</v>
+        <v>44</v>
       </c>
       <c r="G25" s="2" t="n">
-        <v>2859824</v>
+        <v>3013485</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B26" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>48</v>
+      <c r="B26" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="G26" s="2" t="n">
-        <v>3003750</v>
+        <v>2834943</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B27" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="C27" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D27" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="E27" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="F27" s="8" t="s">
-        <v>82</v>
+      <c r="B27" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C27" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="G27" s="2" t="n">
+        <v>2859824</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B28" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D28" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="E28" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="F28" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="G28" s="8" t="s">
-        <v>87</v>
+      <c r="B28" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="G28" s="2" t="n">
+        <v>3003750</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B29" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D29" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="E29" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="F29" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="G29" s="8" t="s">
-        <v>92</v>
+      <c r="B29" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B30" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="C30" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D30" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="E30" s="8" t="s">
+      <c r="B30" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G30" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="F30" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="G30" s="8" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B31" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C31" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="D31" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="E31" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="F31" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="G31" s="7" t="s">
-        <v>100</v>
+      <c r="B31" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B32" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="C32" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D32" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="E32" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="F32" s="8" t="s">
-        <v>102</v>
+      <c r="B32" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1585,277 +1595,271 @@
         <v>1</v>
       </c>
       <c r="B33" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="C33" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D33" s="1" t="s">
+      <c r="C34" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D34" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="E33" s="5" t="s">
+      <c r="E34" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="F33" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="G33" s="2" t="n">
-        <v>1568026</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="B34" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="C34" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D34" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="E34" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="F34" s="7" t="s">
-        <v>111</v>
+      <c r="F34" s="1" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="16.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B35" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>10</v>
+      <c r="B35" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C35" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="D35" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E35" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="E35" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="F35" s="2" t="n">
-        <v>691322110002</v>
+      <c r="F35" s="2" t="s">
+        <v>110</v>
       </c>
       <c r="G35" s="2" t="n">
-        <v>1841315</v>
+        <v>1568026</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="16.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B36" s="7" t="s">
+      <c r="B36" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F36" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="C36" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D36" s="7" t="s">
+      <c r="G36" s="8"/>
+    </row>
+    <row r="37" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A37" s="6"/>
+      <c r="B37" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D37" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="E36" s="7" t="s">
+      <c r="E37" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="F37" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="G37" s="8"/>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A38" s="6"/>
+      <c r="B38" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="C38" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="D38" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="E38" s="9" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B37" s="7" t="s">
+      <c r="F38" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="C37" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D37" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="E37" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="F37" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="G37" s="7" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B38" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="C38" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D38" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="E38" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="F38" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="G38" s="8" t="s">
-        <v>126</v>
-      </c>
+      <c r="G38" s="8"/>
     </row>
     <row r="39" customFormat="false" ht="16.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B39" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="C39" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D39" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="E39" s="8" t="s">
-        <v>129</v>
+      <c r="B39" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="F39" s="2" t="n">
+        <v>691322110002</v>
+      </c>
+      <c r="G39" s="2" t="n">
+        <v>1841315</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="16.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="B40" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="C40" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="D40" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="E40" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="F40" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="G40" s="7" t="s">
-        <v>133</v>
+      <c r="A40" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B41" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="C41" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D41" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="E41" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="F41" s="9" t="s">
-        <v>137</v>
+      <c r="B41" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B42" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="C42" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D42" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="E42" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="F42" s="9" t="s">
-        <v>141</v>
+      <c r="B42" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B43" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="C43" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D43" s="7" t="s">
-        <v>143</v>
-      </c>
-      <c r="E43" s="7" t="s">
-        <v>144</v>
-      </c>
-      <c r="F43" s="7" t="s">
-        <v>143</v>
-      </c>
-      <c r="G43" s="7" t="s">
-        <v>145</v>
+      <c r="B43" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B44" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="C44" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="F44" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="I44" s="1" t="s">
-        <v>149</v>
+      <c r="B44" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="F44" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="G44" s="5" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="C45" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="F45" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="G45" s="2" t="n">
-        <v>3116500</v>
+      <c r="A45" s="6"/>
+      <c r="B45" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D45" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="E45" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="F45" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1863,22 +1867,19 @@
         <v>1</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="C46" s="2" t="n">
-        <v>1</v>
+        <v>141</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="G46" s="2" t="n">
-        <v>2115662</v>
+        <v>144</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1886,22 +1887,19 @@
         <v>1</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="C47" s="2" t="n">
-        <v>1</v>
+        <v>145</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>159</v>
+        <v>146</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>160</v>
+        <v>147</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="G47" s="2" t="n">
-        <v>1578404</v>
+        <v>148</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1909,252 +1907,350 @@
         <v>1</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="F48" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="H48" s="1" t="s">
-        <v>165</v>
+        <v>151</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B49" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="C49" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="D49" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="E49" s="7" t="s">
-        <v>168</v>
-      </c>
-      <c r="F49" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="G49" s="7" t="s">
-        <v>170</v>
+      <c r="B49" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C49" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="I49" s="1" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B50" s="7" t="s">
-        <v>171</v>
-      </c>
-      <c r="C50" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D50" s="7" t="s">
-        <v>172</v>
-      </c>
-      <c r="E50" s="7" t="s">
-        <v>173</v>
-      </c>
-      <c r="F50" s="7" t="s">
-        <v>174</v>
+      <c r="B50" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C50" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="G50" s="2" t="n">
+        <v>3116500</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B51" s="5" t="s">
-        <v>175</v>
-      </c>
-      <c r="C51" s="6" t="s">
-        <v>27</v>
+      <c r="B51" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C51" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>176</v>
+        <v>162</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>177</v>
+        <v>163</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="H51" s="10" t="s">
-        <v>178</v>
-      </c>
-      <c r="I51" s="1" t="s">
-        <v>179</v>
+        <v>164</v>
+      </c>
+      <c r="G51" s="2" t="n">
+        <v>2115662</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B52" s="5" t="s">
+      <c r="B52" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C52" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="G52" s="2" t="n">
+        <v>1578404</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A53" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="F53" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="H53" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A54" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A55" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="E55" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="C52" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="D52" s="1" t="s">
+      <c r="F55" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="E52" s="1" t="s">
+    </row>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A56" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B56" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="F52" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="G52" s="2" t="n">
+      <c r="C56" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="H56" s="11" t="s">
+        <v>185</v>
+      </c>
+      <c r="I56" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A57" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="G57" s="2" t="n">
         <v>1440816</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B53" s="7" t="s">
-        <v>183</v>
-      </c>
-      <c r="C53" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D53" s="7" t="s">
-        <v>184</v>
-      </c>
-      <c r="E53" s="7" t="s">
-        <v>185</v>
-      </c>
-      <c r="F53" s="7" t="s">
-        <v>184</v>
-      </c>
-      <c r="G53" s="7" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="C54" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="E54" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="F54" s="2" t="s">
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A58" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B58" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="G54" s="2" t="n">
+      <c r="C58" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A59" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C59" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="G59" s="2" t="n">
         <v>2308719</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="3"/>
-      <c r="B59" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="D59" s="5" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="11"/>
-      <c r="B60" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="C60" s="2" t="n">
-        <v>5</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="E60" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="F60" s="12" t="s">
-        <v>196</v>
-      </c>
-      <c r="I60" s="1" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="11"/>
-      <c r="B61" s="1" t="s">
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A64" s="3"/>
+      <c r="B64" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="C61" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="D61" s="1" t="s">
+    </row>
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A65" s="3"/>
+      <c r="B65" s="12" t="s">
         <v>199</v>
       </c>
-      <c r="E61" s="1" t="s">
+      <c r="C65" s="13" t="n">
+        <v>4</v>
+      </c>
+      <c r="D65" s="12" t="s">
         <v>200</v>
       </c>
-      <c r="F61" s="12" t="s">
+      <c r="E65" s="12" t="s">
         <v>201</v>
       </c>
-      <c r="I61" s="1" t="s">
+      <c r="F65" s="14" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="11"/>
-      <c r="B62" s="1" t="s">
+      <c r="G65" s="13"/>
+      <c r="I65" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="C62" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D62" s="1" t="s">
+    </row>
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A66" s="3"/>
+      <c r="B66" s="12" t="s">
         <v>204</v>
       </c>
-      <c r="E62" s="1" t="s">
+      <c r="C66" s="13" t="n">
+        <v>3</v>
+      </c>
+      <c r="D66" s="12" t="s">
         <v>205</v>
       </c>
-      <c r="F62" s="12" t="s">
+      <c r="E66" s="12"/>
+      <c r="F66" s="14" t="s">
         <v>206</v>
       </c>
-      <c r="I62" s="1" t="s">
+      <c r="G66" s="13"/>
+      <c r="I66" s="1" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="11"/>
-      <c r="B63" s="1" t="s">
+      <c r="J66" s="0"/>
+    </row>
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A67" s="3"/>
+      <c r="F67" s="15"/>
+    </row>
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A68" s="3"/>
+      <c r="B68" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="C63" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D63" s="1" t="s">
+      <c r="C68" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D68" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="E63" s="1" t="s">
+      <c r="E68" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="F63" s="2" t="s">
+      <c r="F68" s="2" t="s">
         <v>211</v>
       </c>
     </row>
+    <row r="1048532" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048533" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048534" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048535" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2171,7 +2267,7 @@
     <row r="1048546" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048547" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048548" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048549" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048549" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048550" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048551" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048552" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
PCB: layout + BOM + Gerbers ready for review
</commit_message>
<xml_diff>
--- a/pcb/7001-mainboard/7001-ventilator_mainboard.xlsx
+++ b/pcb/7001-mainboard/7001-ventilator_mainboard.xlsx
@@ -598,7 +598,7 @@
     <t xml:space="preserve">LD1086DTTR</t>
   </si>
   <si>
-    <t xml:space="preserve">Package_TO_SOT_SMD:TO-252-2</t>
+    <t xml:space="preserve">Jitter_Footprints:TO-252-2</t>
   </si>
   <si>
     <t xml:space="preserve">LD1086DTTR (adjustable)</t>
@@ -773,7 +773,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -819,6 +819,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -917,8 +921,8 @@
   </sheetPr>
   <dimension ref="A1:I1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B29" activeCellId="0" sqref="B29"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B58" activeCellId="0" sqref="B58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2133,22 +2137,22 @@
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A58" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B58" s="1" t="s">
+      <c r="A58" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="B58" s="12" t="s">
         <v>190</v>
       </c>
-      <c r="C58" s="1" t="s">
+      <c r="C58" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="D58" s="1" t="s">
+      <c r="D58" s="12" t="s">
         <v>191</v>
       </c>
-      <c r="E58" s="1" t="s">
+      <c r="E58" s="12" t="s">
         <v>192</v>
       </c>
-      <c r="F58" s="1" t="s">
+      <c r="F58" s="12" t="s">
         <v>193</v>
       </c>
     </row>
@@ -2186,11 +2190,11 @@
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A65" s="12"/>
+      <c r="A65" s="13"/>
       <c r="B65" s="10" t="s">
         <v>199</v>
       </c>
-      <c r="C65" s="13" t="n">
+      <c r="C65" s="14" t="n">
         <v>4</v>
       </c>
       <c r="D65" s="10" t="s">
@@ -2199,40 +2203,40 @@
       <c r="E65" s="10" t="s">
         <v>201</v>
       </c>
-      <c r="F65" s="14" t="s">
+      <c r="F65" s="15" t="s">
         <v>202</v>
       </c>
-      <c r="G65" s="13"/>
+      <c r="G65" s="14"/>
       <c r="I65" s="1" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A66" s="12"/>
+      <c r="A66" s="13"/>
       <c r="B66" s="10" t="s">
         <v>204</v>
       </c>
-      <c r="C66" s="13" t="n">
+      <c r="C66" s="14" t="n">
         <v>3</v>
       </c>
       <c r="D66" s="10" t="s">
         <v>205</v>
       </c>
       <c r="E66" s="10"/>
-      <c r="F66" s="14" t="s">
+      <c r="F66" s="15" t="s">
         <v>206</v>
       </c>
-      <c r="G66" s="13"/>
+      <c r="G66" s="14"/>
       <c r="I66" s="1" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="3"/>
-      <c r="F67" s="15"/>
-    </row>
-    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A68" s="12"/>
+      <c r="F67" s="16"/>
+    </row>
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="13"/>
       <c r="B68" s="1" t="s">
         <v>208</v>
       </c>
@@ -2249,6 +2253,7 @@
         <v>211</v>
       </c>
     </row>
+    <row r="1048531" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048532" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048533" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048534" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2265,7 +2270,7 @@
     <row r="1048545" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048546" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048547" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048548" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048548" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048549" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048550" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048551" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>